<commit_message>
End of 114 video.
Add basic tank camera controls.
</commit_message>
<xml_diff>
--- a/ControlsTable.xlsx
+++ b/ControlsTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\UE4\UE4 Course Projects\Section_04\04_BattleTank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE7EA9B-5F01-404D-A1C0-C51D3E41C0D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3956DE63-0F49-4EE2-B33D-81716964A091}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
   <si>
     <t>Intention</t>
   </si>
@@ -110,22 +110,56 @@
     <t>Backwards/braking</t>
   </si>
   <si>
-    <t>Left Stick Right</t>
-  </si>
-  <si>
-    <t>D Key</t>
-  </si>
-  <si>
-    <t>Base Rotate left</t>
-  </si>
-  <si>
-    <t>Base Rotate right</t>
-  </si>
-  <si>
     <t>Turret Rotate Left</t>
   </si>
   <si>
     <t>Turret Rotate Right</t>
+  </si>
+  <si>
+    <t>Right Stick Left</t>
+  </si>
+  <si>
+    <t>Right Stick Right</t>
+  </si>
+  <si>
+    <t>Mouse Left</t>
+  </si>
+  <si>
+    <t>Mouse Right</t>
+  </si>
+  <si>
+    <t>Barrel Up</t>
+  </si>
+  <si>
+    <t>Barrel Down</t>
+  </si>
+  <si>
+    <t>Right Stick Down</t>
+  </si>
+  <si>
+    <t>Right Stick Up</t>
+  </si>
+  <si>
+    <t>Mouse  Down</t>
+  </si>
+  <si>
+    <t>Mouse Up</t>
+  </si>
+  <si>
+    <t>Rotate Body Left</t>
+  </si>
+  <si>
+    <t>A-Sym Triggers/
+Bumpers</t>
+  </si>
+  <si>
+    <t>Tracks - Different Speeds</t>
+  </si>
+  <si>
+    <t>Turret Rotator</t>
+  </si>
+  <si>
+    <t>Barrel Elevator</t>
   </si>
 </sst>
 </file>
@@ -173,13 +207,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -188,6 +225,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -528,63 +568,63 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -631,10 +671,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4925E60-2F04-48DC-9E6D-5C0A6A61F71C}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,132 +685,189 @@
     <col min="4" max="4" width="51.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="D8" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7" t="s">
+      <c r="D10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="8"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="9" t="s">
         <v>28</v>
       </c>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{86D1B66A-E386-4AE4-9296-C394AD9AD27A}"/>
-  <mergeCells count="12">
+  <mergeCells count="21">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D14:D15"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
     <mergeCell ref="B6:B7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>